<commit_message>
fixed salvage value calulation issue
</commit_message>
<xml_diff>
--- a/machine_cost_tables.xlsx
+++ b/machine_cost_tables.xlsx
@@ -572,10 +572,10 @@
         <v>200000</v>
       </c>
       <c r="D2">
-        <v>17000</v>
+        <v>40000</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F2">
         <v>1872</v>
@@ -587,7 +587,7 @@
         <v>0.649230769231</v>
       </c>
       <c r="I2">
-        <v>73.294341172</v>
+        <v>56.5070150452</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -601,10 +601,10 @@
         <v>374000</v>
       </c>
       <c r="D3">
-        <v>17000</v>
+        <v>74800</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F3">
         <v>1872</v>
@@ -616,7 +616,7 @@
         <v>0.649230769231</v>
       </c>
       <c r="I3">
-        <v>120.287436828</v>
+        <v>87.3352722135</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -630,7 +630,7 @@
         <v>255000</v>
       </c>
       <c r="D4">
-        <v>17000</v>
+        <v>51000</v>
       </c>
       <c r="E4">
         <v>7.5</v>
@@ -645,7 +645,7 @@
         <v>0.649230769231</v>
       </c>
       <c r="I4">
-        <v>76.2966377139</v>
+        <v>74.7452978886</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -659,7 +659,7 @@
         <v>118056</v>
       </c>
       <c r="D5">
-        <v>17000</v>
+        <v>23611.2</v>
       </c>
       <c r="E5">
         <v>8</v>
@@ -674,7 +674,7 @@
         <v>0.666666666667</v>
       </c>
       <c r="I5">
-        <v>43.4864000665</v>
+        <v>43.2408100045</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -717,7 +717,7 @@
         <v>137949</v>
       </c>
       <c r="D7">
-        <v>30000</v>
+        <v>27589.8</v>
       </c>
       <c r="E7">
         <v>8</v>
@@ -732,7 +732,7 @@
         <v>0.649230769231</v>
       </c>
       <c r="I7">
-        <v>42.6958168686</v>
+        <v>42.7877603491</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -746,7 +746,7 @@
         <v>270000</v>
       </c>
       <c r="D8">
-        <v>30000</v>
+        <v>54000</v>
       </c>
       <c r="E8">
         <v>20</v>
@@ -761,7 +761,7 @@
         <v>0.833333333333</v>
       </c>
       <c r="I8">
-        <v>56.2220111721</v>
+        <v>56.767622612</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -775,7 +775,7 @@
         <v>505000</v>
       </c>
       <c r="D9">
-        <v>30000</v>
+        <v>101000</v>
       </c>
       <c r="E9">
         <v>10</v>
@@ -790,7 +790,7 @@
         <v>0.9375</v>
       </c>
       <c r="I9">
-        <v>100.284909287</v>
+        <v>99.513712625</v>
       </c>
     </row>
   </sheetData>
@@ -837,7 +837,7 @@
         <v>16</v>
       </c>
       <c r="C2">
-        <v>33.1259873618</v>
+        <v>14.4813059505</v>
       </c>
       <c r="D2">
         <v>13.4290440678</v>
@@ -860,7 +860,7 @@
         <v>17</v>
       </c>
       <c r="C3">
-        <v>64.6228278041</v>
+        <v>27.0800421274</v>
       </c>
       <c r="D3">
         <v>16.3666474576</v>
@@ -883,7 +883,7 @@
         <v>18</v>
       </c>
       <c r="C4">
-        <v>28.7212568018</v>
+        <v>24.6182201159</v>
       </c>
       <c r="D4">
         <v>16.7863050847</v>
@@ -906,7 +906,7 @@
         <v>19</v>
       </c>
       <c r="C5">
-        <v>11.133974359</v>
+        <v>10.4055769231</v>
       </c>
       <c r="D5">
         <v>11.5405847458</v>
@@ -952,7 +952,7 @@
         <v>21</v>
       </c>
       <c r="C7">
-        <v>12.2128320004</v>
+        <v>12.485510466</v>
       </c>
       <c r="D7">
         <v>7.2390940678</v>
@@ -975,7 +975,7 @@
         <v>22</v>
       </c>
       <c r="C8">
-        <v>8.46153846154</v>
+        <v>7.61538461538</v>
       </c>
       <c r="D8">
         <v>16.681390678</v>
@@ -998,7 +998,7 @@
         <v>23</v>
       </c>
       <c r="C9">
-        <v>29.7720797721</v>
+        <v>25.3219373219</v>
       </c>
       <c r="D9">
         <v>27.8023177966</v>
@@ -1301,16 +1301,16 @@
         <v>16</v>
       </c>
       <c r="C2">
-        <v>36600</v>
+        <v>16000</v>
       </c>
       <c r="D2">
-        <v>15216</v>
+        <v>15360</v>
       </c>
       <c r="E2">
-        <v>3804</v>
+        <v>3840</v>
       </c>
       <c r="F2">
-        <v>3804</v>
+        <v>3840</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1321,16 +1321,16 @@
         <v>17</v>
       </c>
       <c r="C3">
-        <v>71400</v>
+        <v>29920</v>
       </c>
       <c r="D3">
-        <v>27744</v>
+        <v>28723.2</v>
       </c>
       <c r="E3">
-        <v>6936</v>
+        <v>7180.8</v>
       </c>
       <c r="F3">
-        <v>6936</v>
+        <v>7180.8</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1341,16 +1341,16 @@
         <v>18</v>
       </c>
       <c r="C4">
-        <v>31733.3333333</v>
+        <v>27200</v>
       </c>
       <c r="D4">
-        <v>18224</v>
+        <v>19992</v>
       </c>
       <c r="E4">
-        <v>4556</v>
+        <v>4998</v>
       </c>
       <c r="F4">
-        <v>4556</v>
+        <v>4998</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1361,16 +1361,16 @@
         <v>19</v>
       </c>
       <c r="C5">
-        <v>12632</v>
+        <v>11805.6</v>
       </c>
       <c r="D5">
-        <v>8861.28</v>
+        <v>9208.368</v>
       </c>
       <c r="E5">
-        <v>2215.32</v>
+        <v>2302.092</v>
       </c>
       <c r="F5">
-        <v>2215.32</v>
+        <v>2302.092</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1401,16 +1401,16 @@
         <v>21</v>
       </c>
       <c r="C7">
-        <v>13493.625</v>
+        <v>13794.9</v>
       </c>
       <c r="D7">
-        <v>10886.5575</v>
+        <v>10760.022</v>
       </c>
       <c r="E7">
-        <v>2721.639375</v>
+        <v>2690.0055</v>
       </c>
       <c r="F7">
-        <v>2721.639375</v>
+        <v>2690.0055</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1421,16 +1421,16 @@
         <v>22</v>
       </c>
       <c r="C8">
-        <v>12000</v>
+        <v>10800</v>
       </c>
       <c r="D8">
-        <v>18720</v>
+        <v>20088</v>
       </c>
       <c r="E8">
-        <v>4680</v>
+        <v>5022</v>
       </c>
       <c r="F8">
-        <v>4680</v>
+        <v>5022</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1441,16 +1441,16 @@
         <v>23</v>
       </c>
       <c r="C9">
-        <v>47500</v>
+        <v>40400</v>
       </c>
       <c r="D9">
-        <v>34950</v>
+        <v>38784</v>
       </c>
       <c r="E9">
-        <v>8737.5</v>
+        <v>9696</v>
       </c>
       <c r="F9">
-        <v>8737.5</v>
+        <v>9696</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed nan in tables
</commit_message>
<xml_diff>
--- a/machine_cost_tables.xlsx
+++ b/machine_cost_tables.xlsx
@@ -575,7 +575,7 @@
         <v>40000</v>
       </c>
       <c r="E2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F2">
         <v>1872</v>
@@ -587,7 +587,7 @@
         <v>0.649230769231</v>
       </c>
       <c r="I2">
-        <v>56.5070150452</v>
+        <v>70.8685879997</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -604,7 +604,7 @@
         <v>74800</v>
       </c>
       <c r="E3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F3">
         <v>1872</v>
@@ -616,7 +616,7 @@
         <v>0.649230769231</v>
       </c>
       <c r="I3">
-        <v>87.3352722135</v>
+        <v>114.191413638</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -837,7 +837,7 @@
         <v>16</v>
       </c>
       <c r="C2">
-        <v>14.4813059505</v>
+        <v>28.962611901</v>
       </c>
       <c r="D2">
         <v>13.4290440678</v>
@@ -860,7 +860,7 @@
         <v>17</v>
       </c>
       <c r="C3">
-        <v>27.0800421274</v>
+        <v>54.1600842549</v>
       </c>
       <c r="D3">
         <v>16.3666474576</v>
@@ -1301,16 +1301,16 @@
         <v>16</v>
       </c>
       <c r="C2">
-        <v>16000</v>
+        <v>32000</v>
       </c>
       <c r="D2">
-        <v>15360</v>
+        <v>16320</v>
       </c>
       <c r="E2">
-        <v>3840</v>
+        <v>4080</v>
       </c>
       <c r="F2">
-        <v>3840</v>
+        <v>4080</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1321,16 +1321,16 @@
         <v>17</v>
       </c>
       <c r="C3">
-        <v>29920</v>
+        <v>59840</v>
       </c>
       <c r="D3">
-        <v>28723.2</v>
+        <v>30518.4</v>
       </c>
       <c r="E3">
-        <v>7180.8</v>
+        <v>7629.6</v>
       </c>
       <c r="F3">
-        <v>7180.8</v>
+        <v>7629.6</v>
       </c>
     </row>
     <row r="4" spans="1:6">

</xml_diff>

<commit_message>
Included track/tire replacement costs
Per comment from Tad Mason added tire/track replacement costs. Does not
reflect the replacement schedule however. Several pieces of equipment
have steel tracks and are more expensive but will surely have longer
life. We should add replacement schedule to ensure that costs are reflective.

Changes to be committed:
	modified:   EquipCost.csv
	modified:   hfrd_machinecost.db
	modified:   hfrd_pmh.py
	modified:   machine_cost_tables.xlsx
	modified:   results.md
</commit_message>
<xml_diff>
--- a/machine_cost_tables.xlsx
+++ b/machine_cost_tables.xlsx
@@ -130,21 +130,10 @@
     <t xml:space="preserve">Mobile walking excavator, machine works on steep slopes ranging from 30-60 degrees. </t>
   </si>
   <si>
-    <t>Prime Tech PT-175 Dedicated Carrier with FAE 140/U/ST-175 Mulching head with C-type teeth.
-Mechanical push-frame with guide pins for 140/U-175
-Rear winch with 5.6 t pulling power
-Rear view camera, with extra display
-Comfort driver's seat (heated and with pneumatic suspension)
-Reversible fan for the engine radiator (including compressor)
-Additional handle for emergency exit (to open it up from the outside)
-All cab windows in 12mm Lexan Margard
-Rock guards for lower rollers
-STD-500 mm tracks-single grouser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Takeuchi TL12 high flow track loader with FAE UML/SSL/VT-150 mastication head, with tooth type C/3 (standard)
-TL12 with ROPS/FOPS Cab with air conditioning/Heat, Defroster, 17.7" rubber tracks, hydraulic quick attach, roll up Lexan door, High Flow Auxiliary Hydraulics w/second auxiliary line.
-FAE UML/SSL/VT-150 Universal forestry mulcher for skid steer with push-frame. </t>
+    <t>Prime Tech PT-175 Dedicated Carrier with FAE 140/U/ST-175 Mulching head with C-type teeth._x000D__x000D_Mechanical push-frame with guide pins for 140/U-175_x000D_Rear winch with 5.6 t pulling power_x000D_Rear view camera, with extra display_x000D_Comfort driver's seat (heated and with pneumatic suspension)_x000D_Reversible fan for the engine radiator (including compressor)_x000D_Additional handle for emergency exit (to open it up from the outside)_x000D_All cab windows in 12mm Lexan Margard_x000D_Rock guards for lower rollers_x000D_STD-500 mm tracks-single grouser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Takeuchi TL12 high flow track loader with FAE UML/SSL/VT-150 mastication head, with tooth type C/3 (standard)_x000D__x000D_TL12 with ROPS/FOPS Cab with air conditioning/Heat, Defroster, 17.7" rubber tracks, hydraulic quick attach, roll up Lexan door, High Flow Auxiliary Hydraulics w/second auxiliary line._x000D__x000D_FAE UML/SSL/VT-150 Universal forestry mulcher for skid steer with push-frame. </t>
   </si>
   <si>
     <t>Cat High Flow Compact Track Loader for use in high demand applications. This is a steel track machine (optional) vs rubber belt. Also included is a HM415B designed specificially for the host machine.</t>
@@ -587,7 +576,7 @@
         <v>0.649230769231</v>
       </c>
       <c r="I2">
-        <v>70.8685879997</v>
+        <v>74.1269213331</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -616,7 +605,7 @@
         <v>0.649230769231</v>
       </c>
       <c r="I3">
-        <v>114.191413638</v>
+        <v>115.763080305</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -645,7 +634,7 @@
         <v>0.649230769231</v>
       </c>
       <c r="I4">
-        <v>74.7452978886</v>
+        <v>74.55363122200001</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -674,7 +663,7 @@
         <v>0.666666666667</v>
       </c>
       <c r="I5">
-        <v>43.2408100045</v>
+        <v>43.0491433378</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -703,7 +692,7 @@
         <v>0.649230769231</v>
       </c>
       <c r="I6">
-        <v>57.2749783662</v>
+        <v>61.1466450328</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -732,7 +721,7 @@
         <v>0.649230769231</v>
       </c>
       <c r="I7">
-        <v>42.7877603491</v>
+        <v>42.5960936825</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -761,7 +750,7 @@
         <v>0.833333333333</v>
       </c>
       <c r="I8">
-        <v>56.767622612</v>
+        <v>61.942622612</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -790,7 +779,7 @@
         <v>0.9375</v>
       </c>
       <c r="I9">
-        <v>99.513712625</v>
+        <v>101.813712625</v>
       </c>
     </row>
   </sheetData>
@@ -846,7 +835,7 @@
         <v>0.0326851351351</v>
       </c>
       <c r="F2">
-        <v>0.575</v>
+        <v>3.83333333333</v>
       </c>
       <c r="G2">
         <v>15.82</v>
@@ -869,7 +858,7 @@
         <v>0.0106851351351</v>
       </c>
       <c r="F3">
-        <v>0.575</v>
+        <v>2.14666666667</v>
       </c>
       <c r="G3">
         <v>15.82</v>
@@ -892,7 +881,7 @@
         <v>0.0128451351351</v>
       </c>
       <c r="F4">
-        <v>0.575</v>
+        <v>0.383333333333</v>
       </c>
       <c r="G4">
         <v>15.82</v>
@@ -915,7 +904,7 @@
         <v>0.0142851351351</v>
       </c>
       <c r="F5">
-        <v>0.575</v>
+        <v>0.383333333333</v>
       </c>
       <c r="G5">
         <v>15.82</v>
@@ -938,7 +927,7 @@
         <v>0.0146851351351</v>
       </c>
       <c r="F6">
-        <v>0.575</v>
+        <v>4.44666666667</v>
       </c>
       <c r="G6">
         <v>15.82</v>
@@ -961,7 +950,7 @@
         <v>0.0206851351351</v>
       </c>
       <c r="F7">
-        <v>0.575</v>
+        <v>0.383333333333</v>
       </c>
       <c r="G7">
         <v>15.82</v>
@@ -984,7 +973,7 @@
         <v>0.0281851351351</v>
       </c>
       <c r="F8">
-        <v>0.575</v>
+        <v>5.75</v>
       </c>
       <c r="G8">
         <v>15.82</v>
@@ -1007,7 +996,7 @@
         <v>0.0406851351351</v>
       </c>
       <c r="F9">
-        <v>0.575</v>
+        <v>2.875</v>
       </c>
       <c r="G9">
         <v>15.82</v>

</xml_diff>

<commit_message>
Added track replacement schedule.
Per email from Brian Kile #1 track replacement schedules have been
modified. Still need to confirm replacement schedule for PrimeTech as
current schedule is the same as rubber-tracked units.

	modified:   EquipCost.csv
	modified:   hfrd_machinecost.db
	modified:   hfrd_pmh.py
	modified:   machine_cost_tables.xlsx
	modified:   results.md
</commit_message>
<xml_diff>
--- a/machine_cost_tables.xlsx
+++ b/machine_cost_tables.xlsx
@@ -576,7 +576,7 @@
         <v>0.649230769231</v>
       </c>
       <c r="I2">
-        <v>74.1269213331</v>
+        <v>74.3185879997</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -634,7 +634,7 @@
         <v>0.649230769231</v>
       </c>
       <c r="I4">
-        <v>74.55363122200001</v>
+        <v>76.4702978886</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -663,7 +663,7 @@
         <v>0.666666666667</v>
       </c>
       <c r="I5">
-        <v>43.0491433378</v>
+        <v>44.9658100045</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -692,7 +692,7 @@
         <v>0.649230769231</v>
       </c>
       <c r="I6">
-        <v>61.1466450328</v>
+        <v>59.3833116995</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -721,7 +721,7 @@
         <v>0.649230769231</v>
       </c>
       <c r="I7">
-        <v>42.5960936825</v>
+        <v>44.5127603491</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -750,7 +750,7 @@
         <v>0.833333333333</v>
       </c>
       <c r="I8">
-        <v>61.942622612</v>
+        <v>60.505122612</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -779,7 +779,7 @@
         <v>0.9375</v>
       </c>
       <c r="I9">
-        <v>101.813712625</v>
+        <v>101.094962625</v>
       </c>
     </row>
   </sheetData>
@@ -835,7 +835,7 @@
         <v>0.0326851351351</v>
       </c>
       <c r="F2">
-        <v>3.83333333333</v>
+        <v>4.025</v>
       </c>
       <c r="G2">
         <v>15.82</v>
@@ -881,7 +881,7 @@
         <v>0.0128451351351</v>
       </c>
       <c r="F4">
-        <v>0.383333333333</v>
+        <v>2.3</v>
       </c>
       <c r="G4">
         <v>15.82</v>
@@ -904,7 +904,7 @@
         <v>0.0142851351351</v>
       </c>
       <c r="F5">
-        <v>0.383333333333</v>
+        <v>2.3</v>
       </c>
       <c r="G5">
         <v>15.82</v>
@@ -927,7 +927,7 @@
         <v>0.0146851351351</v>
       </c>
       <c r="F6">
-        <v>4.44666666667</v>
+        <v>2.68333333333</v>
       </c>
       <c r="G6">
         <v>15.82</v>
@@ -950,7 +950,7 @@
         <v>0.0206851351351</v>
       </c>
       <c r="F7">
-        <v>0.383333333333</v>
+        <v>2.3</v>
       </c>
       <c r="G7">
         <v>15.82</v>
@@ -973,7 +973,7 @@
         <v>0.0281851351351</v>
       </c>
       <c r="F8">
-        <v>5.75</v>
+        <v>4.3125</v>
       </c>
       <c r="G8">
         <v>15.82</v>
@@ -996,7 +996,7 @@
         <v>0.0406851351351</v>
       </c>
       <c r="F9">
-        <v>2.875</v>
+        <v>2.15625</v>
       </c>
       <c r="G9">
         <v>15.82</v>

</xml_diff>